<commit_message>
[V&V] Aplicação dos artefatos RT, RAVV, RGA, PLA-VER-VAL
</commit_message>
<xml_diff>
--- a/Artefatos de Documentação/Processo Aplicado/EveRemind/6-Verificacao e Validacao/Casos de Teste.xlsx
+++ b/Artefatos de Documentação/Processo Aplicado/EveRemind/6-Verificacao e Validacao/Casos de Teste.xlsx
@@ -1491,6 +1491,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1502,99 +1505,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="52">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="40">
     <dxf>
       <fill>
         <patternFill>
@@ -2153,7 +2069,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="L103" sqref="L103"/>
     </sheetView>
   </sheetViews>
@@ -2196,13 +2112,13 @@
       </c>
     </row>
     <row r="2" spans="1:8" s="1" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="13" t="s">
         <v>302</v>
       </c>
       <c r="D2" s="3" t="s">
@@ -2222,9 +2138,9 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A3" s="13"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
+      <c r="A3" s="14"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
       <c r="D3" s="5" t="s">
         <v>12</v>
       </c>
@@ -2240,9 +2156,9 @@
       <c r="H3" s="5"/>
     </row>
     <row r="4" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A4" s="13"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
+      <c r="A4" s="14"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
       <c r="D4" s="5" t="s">
         <v>13</v>
       </c>
@@ -2258,9 +2174,9 @@
       <c r="H4" s="5"/>
     </row>
     <row r="5" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
+      <c r="A5" s="14"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
       <c r="D5" s="5" t="s">
         <v>14</v>
       </c>
@@ -2276,9 +2192,9 @@
       <c r="H5" s="5"/>
     </row>
     <row r="6" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A6" s="13"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
+      <c r="A6" s="14"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
       <c r="D6" s="5" t="s">
         <v>15</v>
       </c>
@@ -2294,9 +2210,9 @@
       <c r="H6" s="5"/>
     </row>
     <row r="7" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" s="13"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
+      <c r="A7" s="14"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
       <c r="D7" s="5" t="s">
         <v>20</v>
       </c>
@@ -2312,9 +2228,9 @@
       <c r="H7" s="5"/>
     </row>
     <row r="8" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A8" s="13"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
+      <c r="A8" s="14"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
       <c r="D8" s="5" t="s">
         <v>21</v>
       </c>
@@ -2330,9 +2246,9 @@
       <c r="H8" s="5"/>
     </row>
     <row r="9" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
+      <c r="A9" s="14"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
       <c r="D9" s="5" t="s">
         <v>22</v>
       </c>
@@ -2348,9 +2264,9 @@
       <c r="H9" s="5"/>
     </row>
     <row r="10" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A10" s="13"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
+      <c r="A10" s="14"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
       <c r="D10" s="5" t="s">
         <v>23</v>
       </c>
@@ -2366,9 +2282,9 @@
       <c r="H10" s="5"/>
     </row>
     <row r="11" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A11" s="13"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
+      <c r="A11" s="14"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
       <c r="D11" s="5" t="s">
         <v>26</v>
       </c>
@@ -2384,9 +2300,9 @@
       <c r="H11" s="5"/>
     </row>
     <row r="12" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A12" s="13"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
+      <c r="A12" s="14"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
       <c r="D12" s="5" t="s">
         <v>28</v>
       </c>
@@ -2402,9 +2318,9 @@
       <c r="H12" s="7"/>
     </row>
     <row r="13" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A13" s="13"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
+      <c r="A13" s="14"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
       <c r="D13" s="5" t="s">
         <v>29</v>
       </c>
@@ -2420,9 +2336,9 @@
       <c r="H13" s="5"/>
     </row>
     <row r="14" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A14" s="13"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="13"/>
+      <c r="A14" s="14"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
       <c r="D14" s="5" t="s">
         <v>32</v>
       </c>
@@ -2438,9 +2354,9 @@
       <c r="H14" s="5"/>
     </row>
     <row r="15" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A15" s="13"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
+      <c r="A15" s="14"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
       <c r="D15" s="5" t="s">
         <v>34</v>
       </c>
@@ -2456,9 +2372,9 @@
       <c r="H15" s="5"/>
     </row>
     <row r="16" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A16" s="13"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
+      <c r="A16" s="14"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
       <c r="D16" s="5" t="s">
         <v>34</v>
       </c>
@@ -2474,9 +2390,9 @@
       <c r="H16" s="5"/>
     </row>
     <row r="17" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A17" s="13"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="13"/>
+      <c r="A17" s="14"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
       <c r="D17" s="5" t="s">
         <v>35</v>
       </c>
@@ -2492,9 +2408,9 @@
       <c r="H17" s="5"/>
     </row>
     <row r="18" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A18" s="13"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="13"/>
+      <c r="A18" s="14"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
       <c r="D18" s="5" t="s">
         <v>35</v>
       </c>
@@ -2510,9 +2426,9 @@
       <c r="H18" s="5"/>
     </row>
     <row r="19" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A19" s="13"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="13"/>
+      <c r="A19" s="14"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
       <c r="D19" s="5" t="s">
         <v>36</v>
       </c>
@@ -2528,9 +2444,9 @@
       <c r="H19" s="5"/>
     </row>
     <row r="20" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A20" s="13"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="13"/>
+      <c r="A20" s="14"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
       <c r="D20" s="5" t="s">
         <v>37</v>
       </c>
@@ -2546,9 +2462,9 @@
       <c r="H20" s="5"/>
     </row>
     <row r="21" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A21" s="13"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="13"/>
+      <c r="A21" s="14"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
       <c r="D21" s="5" t="s">
         <v>37</v>
       </c>
@@ -2564,9 +2480,9 @@
       <c r="H21" s="5"/>
     </row>
     <row r="22" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A22" s="13"/>
-      <c r="B22" s="13"/>
-      <c r="C22" s="13"/>
+      <c r="A22" s="14"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="14"/>
       <c r="D22" s="5" t="s">
         <v>47</v>
       </c>
@@ -2582,9 +2498,9 @@
       <c r="H22" s="5"/>
     </row>
     <row r="23" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A23" s="13"/>
-      <c r="B23" s="13"/>
-      <c r="C23" s="13"/>
+      <c r="A23" s="14"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="14"/>
       <c r="D23" s="5" t="s">
         <v>48</v>
       </c>
@@ -2600,9 +2516,9 @@
       <c r="H23" s="5"/>
     </row>
     <row r="24" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A24" s="13"/>
-      <c r="B24" s="13"/>
-      <c r="C24" s="13"/>
+      <c r="A24" s="14"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="14"/>
       <c r="D24" s="5" t="s">
         <v>49</v>
       </c>
@@ -2618,9 +2534,9 @@
       <c r="H24" s="5"/>
     </row>
     <row r="25" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A25" s="13"/>
-      <c r="B25" s="13"/>
-      <c r="C25" s="14"/>
+      <c r="A25" s="14"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="15"/>
       <c r="D25" s="5" t="s">
         <v>50</v>
       </c>
@@ -2636,9 +2552,9 @@
       <c r="H25" s="5"/>
     </row>
     <row r="26" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A26" s="13"/>
-      <c r="B26" s="13"/>
-      <c r="C26" s="12" t="s">
+      <c r="A26" s="14"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="13" t="s">
         <v>332</v>
       </c>
       <c r="D26" s="5" t="s">
@@ -2656,9 +2572,9 @@
       <c r="H26" s="5"/>
     </row>
     <row r="27" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A27" s="14"/>
-      <c r="B27" s="14"/>
-      <c r="C27" s="14"/>
+      <c r="A27" s="15"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="15"/>
       <c r="D27" s="5" t="s">
         <v>56</v>
       </c>
@@ -2674,13 +2590,13 @@
       <c r="H27" s="5"/>
     </row>
     <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="12" t="s">
+      <c r="A28" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="B28" s="12" t="s">
+      <c r="B28" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="C28" s="12" t="s">
+      <c r="C28" s="13" t="s">
         <v>322</v>
       </c>
       <c r="D28" s="5" t="s">
@@ -2698,9 +2614,9 @@
       <c r="H28" s="3"/>
     </row>
     <row r="29" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="13"/>
-      <c r="B29" s="13"/>
-      <c r="C29" s="13"/>
+      <c r="A29" s="14"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="14"/>
       <c r="D29" s="5" t="s">
         <v>69</v>
       </c>
@@ -2716,9 +2632,9 @@
       <c r="H29" s="3"/>
     </row>
     <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="13"/>
-      <c r="B30" s="13"/>
-      <c r="C30" s="13"/>
+      <c r="A30" s="14"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="14"/>
       <c r="D30" s="5" t="s">
         <v>70</v>
       </c>
@@ -2734,9 +2650,9 @@
       <c r="H30" s="3"/>
     </row>
     <row r="31" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="13"/>
-      <c r="B31" s="13"/>
-      <c r="C31" s="13"/>
+      <c r="A31" s="14"/>
+      <c r="B31" s="14"/>
+      <c r="C31" s="14"/>
       <c r="D31" s="5" t="s">
         <v>71</v>
       </c>
@@ -2752,9 +2668,9 @@
       <c r="H31" s="3"/>
     </row>
     <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="13"/>
-      <c r="B32" s="13"/>
-      <c r="C32" s="13"/>
+      <c r="A32" s="14"/>
+      <c r="B32" s="14"/>
+      <c r="C32" s="14"/>
       <c r="D32" s="5" t="s">
         <v>72</v>
       </c>
@@ -2770,9 +2686,9 @@
       <c r="H32" s="3"/>
     </row>
     <row r="33" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="13"/>
-      <c r="B33" s="13"/>
-      <c r="C33" s="13"/>
+      <c r="A33" s="14"/>
+      <c r="B33" s="14"/>
+      <c r="C33" s="14"/>
       <c r="D33" s="5" t="s">
         <v>73</v>
       </c>
@@ -2788,9 +2704,9 @@
       <c r="H33" s="3"/>
     </row>
     <row r="34" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="14"/>
-      <c r="B34" s="14"/>
-      <c r="C34" s="14"/>
+      <c r="A34" s="15"/>
+      <c r="B34" s="15"/>
+      <c r="C34" s="15"/>
       <c r="D34" s="5" t="s">
         <v>74</v>
       </c>
@@ -2806,13 +2722,13 @@
       <c r="H34" s="3"/>
     </row>
     <row r="35" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A35" s="12" t="s">
+      <c r="A35" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="B35" s="12" t="s">
+      <c r="B35" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="C35" s="12" t="s">
+      <c r="C35" s="13" t="s">
         <v>324</v>
       </c>
       <c r="D35" s="5" t="s">
@@ -2830,9 +2746,9 @@
       <c r="H35" s="4"/>
     </row>
     <row r="36" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A36" s="13"/>
-      <c r="B36" s="13"/>
-      <c r="C36" s="13"/>
+      <c r="A36" s="14"/>
+      <c r="B36" s="14"/>
+      <c r="C36" s="14"/>
       <c r="D36" s="5" t="s">
         <v>85</v>
       </c>
@@ -2848,9 +2764,9 @@
       <c r="H36" s="6"/>
     </row>
     <row r="37" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A37" s="13"/>
-      <c r="B37" s="13"/>
-      <c r="C37" s="13"/>
+      <c r="A37" s="14"/>
+      <c r="B37" s="14"/>
+      <c r="C37" s="14"/>
       <c r="D37" s="5" t="s">
         <v>86</v>
       </c>
@@ -2866,9 +2782,9 @@
       <c r="H37" s="5"/>
     </row>
     <row r="38" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A38" s="13"/>
-      <c r="B38" s="13"/>
-      <c r="C38" s="13"/>
+      <c r="A38" s="14"/>
+      <c r="B38" s="14"/>
+      <c r="C38" s="14"/>
       <c r="D38" s="5" t="s">
         <v>87</v>
       </c>
@@ -2884,9 +2800,9 @@
       <c r="H38" s="5"/>
     </row>
     <row r="39" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A39" s="13"/>
-      <c r="B39" s="13"/>
-      <c r="C39" s="13"/>
+      <c r="A39" s="14"/>
+      <c r="B39" s="14"/>
+      <c r="C39" s="14"/>
       <c r="D39" s="5" t="s">
         <v>88</v>
       </c>
@@ -2902,9 +2818,9 @@
       <c r="H39" s="5"/>
     </row>
     <row r="40" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A40" s="13"/>
-      <c r="B40" s="13"/>
-      <c r="C40" s="13"/>
+      <c r="A40" s="14"/>
+      <c r="B40" s="14"/>
+      <c r="C40" s="14"/>
       <c r="D40" s="5" t="s">
         <v>94</v>
       </c>
@@ -2922,9 +2838,9 @@
       </c>
     </row>
     <row r="41" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A41" s="13"/>
-      <c r="B41" s="13"/>
-      <c r="C41" s="13"/>
+      <c r="A41" s="14"/>
+      <c r="B41" s="14"/>
+      <c r="C41" s="14"/>
       <c r="D41" s="5" t="s">
         <v>95</v>
       </c>
@@ -2942,9 +2858,9 @@
       </c>
     </row>
     <row r="42" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A42" s="13"/>
-      <c r="B42" s="13"/>
-      <c r="C42" s="13"/>
+      <c r="A42" s="14"/>
+      <c r="B42" s="14"/>
+      <c r="C42" s="14"/>
       <c r="D42" s="5" t="s">
         <v>96</v>
       </c>
@@ -2962,9 +2878,9 @@
       </c>
     </row>
     <row r="43" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A43" s="13"/>
-      <c r="B43" s="13"/>
-      <c r="C43" s="13"/>
+      <c r="A43" s="14"/>
+      <c r="B43" s="14"/>
+      <c r="C43" s="14"/>
       <c r="D43" s="5" t="s">
         <v>102</v>
       </c>
@@ -2982,9 +2898,9 @@
       </c>
     </row>
     <row r="44" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A44" s="13"/>
-      <c r="B44" s="13"/>
-      <c r="C44" s="13"/>
+      <c r="A44" s="14"/>
+      <c r="B44" s="14"/>
+      <c r="C44" s="14"/>
       <c r="D44" s="5" t="s">
         <v>103</v>
       </c>
@@ -3000,9 +2916,9 @@
       <c r="H44" s="5"/>
     </row>
     <row r="45" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A45" s="13"/>
-      <c r="B45" s="14"/>
-      <c r="C45" s="14"/>
+      <c r="A45" s="14"/>
+      <c r="B45" s="15"/>
+      <c r="C45" s="15"/>
       <c r="D45" s="5" t="s">
         <v>105</v>
       </c>
@@ -3018,11 +2934,11 @@
       <c r="H45" s="5"/>
     </row>
     <row r="46" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A46" s="13"/>
-      <c r="B46" s="12" t="s">
+      <c r="A46" s="14"/>
+      <c r="B46" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="C46" s="12" t="s">
+      <c r="C46" s="13" t="s">
         <v>101</v>
       </c>
       <c r="D46" s="5" t="s">
@@ -3040,9 +2956,9 @@
       <c r="H46" s="9"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="13"/>
-      <c r="B47" s="13"/>
-      <c r="C47" s="13"/>
+      <c r="A47" s="14"/>
+      <c r="B47" s="14"/>
+      <c r="C47" s="14"/>
       <c r="D47" s="5" t="s">
         <v>110</v>
       </c>
@@ -3058,9 +2974,9 @@
       <c r="H47" s="9"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="13"/>
-      <c r="B48" s="13"/>
-      <c r="C48" s="13"/>
+      <c r="A48" s="14"/>
+      <c r="B48" s="14"/>
+      <c r="C48" s="14"/>
       <c r="D48" s="5" t="s">
         <v>112</v>
       </c>
@@ -3076,9 +2992,9 @@
       <c r="H48" s="9"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="13"/>
-      <c r="B49" s="13"/>
-      <c r="C49" s="13"/>
+      <c r="A49" s="14"/>
+      <c r="B49" s="14"/>
+      <c r="C49" s="14"/>
       <c r="D49" s="5" t="s">
         <v>115</v>
       </c>
@@ -3094,9 +3010,9 @@
       <c r="H49" s="9"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="13"/>
-      <c r="B50" s="13"/>
-      <c r="C50" s="13"/>
+      <c r="A50" s="14"/>
+      <c r="B50" s="14"/>
+      <c r="C50" s="14"/>
       <c r="D50" s="5" t="s">
         <v>116</v>
       </c>
@@ -3112,9 +3028,9 @@
       <c r="H50" s="5"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="13"/>
-      <c r="B51" s="13"/>
-      <c r="C51" s="13"/>
+      <c r="A51" s="14"/>
+      <c r="B51" s="14"/>
+      <c r="C51" s="14"/>
       <c r="D51" s="5" t="s">
         <v>117</v>
       </c>
@@ -3130,9 +3046,9 @@
       <c r="H51" s="5"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="13"/>
-      <c r="B52" s="14"/>
-      <c r="C52" s="14"/>
+      <c r="A52" s="14"/>
+      <c r="B52" s="15"/>
+      <c r="C52" s="15"/>
       <c r="D52" s="5" t="s">
         <v>118</v>
       </c>
@@ -3148,11 +3064,11 @@
       <c r="H52" s="5"/>
     </row>
     <row r="53" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="13"/>
-      <c r="B53" s="12" t="s">
+      <c r="A53" s="14"/>
+      <c r="B53" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="C53" s="12" t="s">
+      <c r="C53" s="13" t="s">
         <v>122</v>
       </c>
       <c r="D53" s="5" t="s">
@@ -3170,9 +3086,9 @@
       <c r="H53" s="9"/>
     </row>
     <row r="54" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A54" s="13"/>
-      <c r="B54" s="13"/>
-      <c r="C54" s="13"/>
+      <c r="A54" s="14"/>
+      <c r="B54" s="14"/>
+      <c r="C54" s="14"/>
       <c r="D54" s="5" t="s">
         <v>120</v>
       </c>
@@ -3188,9 +3104,9 @@
       <c r="H54" s="5"/>
     </row>
     <row r="55" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A55" s="13"/>
-      <c r="B55" s="13"/>
-      <c r="C55" s="13"/>
+      <c r="A55" s="14"/>
+      <c r="B55" s="14"/>
+      <c r="C55" s="14"/>
       <c r="D55" s="5" t="s">
         <v>121</v>
       </c>
@@ -3206,9 +3122,9 @@
       <c r="H55" s="5"/>
     </row>
     <row r="56" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A56" s="13"/>
-      <c r="B56" s="13"/>
-      <c r="C56" s="13"/>
+      <c r="A56" s="14"/>
+      <c r="B56" s="14"/>
+      <c r="C56" s="14"/>
       <c r="D56" s="5" t="s">
         <v>134</v>
       </c>
@@ -3224,9 +3140,9 @@
       <c r="H56" s="5"/>
     </row>
     <row r="57" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A57" s="13"/>
-      <c r="B57" s="13"/>
-      <c r="C57" s="13"/>
+      <c r="A57" s="14"/>
+      <c r="B57" s="14"/>
+      <c r="C57" s="14"/>
       <c r="D57" s="5" t="s">
         <v>135</v>
       </c>
@@ -3242,9 +3158,9 @@
       <c r="H57" s="5"/>
     </row>
     <row r="58" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A58" s="13"/>
-      <c r="B58" s="13"/>
-      <c r="C58" s="13"/>
+      <c r="A58" s="14"/>
+      <c r="B58" s="14"/>
+      <c r="C58" s="14"/>
       <c r="D58" s="5" t="s">
         <v>136</v>
       </c>
@@ -3260,9 +3176,9 @@
       <c r="H58" s="5"/>
     </row>
     <row r="59" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="13"/>
-      <c r="B59" s="13"/>
-      <c r="C59" s="13"/>
+      <c r="A59" s="14"/>
+      <c r="B59" s="14"/>
+      <c r="C59" s="14"/>
       <c r="D59" s="5" t="s">
         <v>137</v>
       </c>
@@ -3278,11 +3194,11 @@
       <c r="H59" s="5"/>
     </row>
     <row r="60" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="13"/>
-      <c r="B60" s="12" t="s">
+      <c r="A60" s="14"/>
+      <c r="B60" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="C60" s="12" t="s">
+      <c r="C60" s="13" t="s">
         <v>127</v>
       </c>
       <c r="D60" s="5" t="s">
@@ -3300,9 +3216,9 @@
       <c r="H60" s="5"/>
     </row>
     <row r="61" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A61" s="13"/>
-      <c r="B61" s="13"/>
-      <c r="C61" s="13"/>
+      <c r="A61" s="14"/>
+      <c r="B61" s="14"/>
+      <c r="C61" s="14"/>
       <c r="D61" s="5" t="s">
         <v>150</v>
       </c>
@@ -3318,9 +3234,9 @@
       <c r="H61" s="5"/>
     </row>
     <row r="62" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A62" s="13"/>
-      <c r="B62" s="13"/>
-      <c r="C62" s="13"/>
+      <c r="A62" s="14"/>
+      <c r="B62" s="14"/>
+      <c r="C62" s="14"/>
       <c r="D62" s="5" t="s">
         <v>151</v>
       </c>
@@ -3336,9 +3252,9 @@
       <c r="H62" s="5"/>
     </row>
     <row r="63" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A63" s="13"/>
-      <c r="B63" s="13"/>
-      <c r="C63" s="13"/>
+      <c r="A63" s="14"/>
+      <c r="B63" s="14"/>
+      <c r="C63" s="14"/>
       <c r="D63" s="5" t="s">
         <v>156</v>
       </c>
@@ -3354,9 +3270,9 @@
       <c r="H63" s="5"/>
     </row>
     <row r="64" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A64" s="13"/>
-      <c r="B64" s="13"/>
-      <c r="C64" s="13"/>
+      <c r="A64" s="14"/>
+      <c r="B64" s="14"/>
+      <c r="C64" s="14"/>
       <c r="D64" s="5" t="s">
         <v>157</v>
       </c>
@@ -3372,9 +3288,9 @@
       <c r="H64" s="5"/>
     </row>
     <row r="65" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A65" s="13"/>
-      <c r="B65" s="13"/>
-      <c r="C65" s="13"/>
+      <c r="A65" s="14"/>
+      <c r="B65" s="14"/>
+      <c r="C65" s="14"/>
       <c r="D65" s="5" t="s">
         <v>158</v>
       </c>
@@ -3390,9 +3306,9 @@
       <c r="H65" s="5"/>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A66" s="13"/>
-      <c r="B66" s="14"/>
-      <c r="C66" s="14"/>
+      <c r="A66" s="14"/>
+      <c r="B66" s="15"/>
+      <c r="C66" s="15"/>
       <c r="D66" s="5" t="s">
         <v>159</v>
       </c>
@@ -3408,11 +3324,11 @@
       <c r="H66" s="5"/>
     </row>
     <row r="67" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="13"/>
-      <c r="B67" s="12" t="s">
+      <c r="A67" s="14"/>
+      <c r="B67" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="C67" s="12" t="s">
+      <c r="C67" s="13" t="s">
         <v>146</v>
       </c>
       <c r="D67" s="5" t="s">
@@ -3430,9 +3346,9 @@
       <c r="H67" s="5"/>
     </row>
     <row r="68" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A68" s="13"/>
-      <c r="B68" s="13"/>
-      <c r="C68" s="13"/>
+      <c r="A68" s="14"/>
+      <c r="B68" s="14"/>
+      <c r="C68" s="14"/>
       <c r="D68" s="5" t="s">
         <v>167</v>
       </c>
@@ -3448,9 +3364,9 @@
       <c r="H68" s="5"/>
     </row>
     <row r="69" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A69" s="13"/>
-      <c r="B69" s="13"/>
-      <c r="C69" s="13"/>
+      <c r="A69" s="14"/>
+      <c r="B69" s="14"/>
+      <c r="C69" s="14"/>
       <c r="D69" s="5" t="s">
         <v>171</v>
       </c>
@@ -3466,9 +3382,9 @@
       <c r="H69" s="5"/>
     </row>
     <row r="70" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="13"/>
-      <c r="B70" s="13"/>
-      <c r="C70" s="13"/>
+      <c r="A70" s="14"/>
+      <c r="B70" s="14"/>
+      <c r="C70" s="14"/>
       <c r="D70" s="5" t="s">
         <v>174</v>
       </c>
@@ -3484,9 +3400,9 @@
       <c r="H70" s="5"/>
     </row>
     <row r="71" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A71" s="14"/>
-      <c r="B71" s="14"/>
-      <c r="C71" s="14"/>
+      <c r="A71" s="15"/>
+      <c r="B71" s="15"/>
+      <c r="C71" s="15"/>
       <c r="D71" s="5" t="s">
         <v>175</v>
       </c>
@@ -3502,13 +3418,13 @@
       <c r="H71" s="5"/>
     </row>
     <row r="72" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="12" t="s">
+      <c r="A72" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="B72" s="12" t="s">
+      <c r="B72" s="13" t="s">
         <v>155</v>
       </c>
-      <c r="C72" s="12" t="s">
+      <c r="C72" s="13" t="s">
         <v>173</v>
       </c>
       <c r="D72" s="5" t="s">
@@ -3526,9 +3442,9 @@
       <c r="H72" s="5"/>
     </row>
     <row r="73" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A73" s="13"/>
-      <c r="B73" s="13"/>
-      <c r="C73" s="13"/>
+      <c r="A73" s="14"/>
+      <c r="B73" s="14"/>
+      <c r="C73" s="14"/>
       <c r="D73" s="5" t="s">
         <v>177</v>
       </c>
@@ -3544,9 +3460,9 @@
       <c r="H73" s="5"/>
     </row>
     <row r="74" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A74" s="13"/>
-      <c r="B74" s="13"/>
-      <c r="C74" s="13"/>
+      <c r="A74" s="14"/>
+      <c r="B74" s="14"/>
+      <c r="C74" s="14"/>
       <c r="D74" s="5" t="s">
         <v>183</v>
       </c>
@@ -3562,9 +3478,9 @@
       <c r="H74" s="5"/>
     </row>
     <row r="75" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A75" s="13"/>
-      <c r="B75" s="13"/>
-      <c r="C75" s="13"/>
+      <c r="A75" s="14"/>
+      <c r="B75" s="14"/>
+      <c r="C75" s="14"/>
       <c r="D75" s="5" t="s">
         <v>184</v>
       </c>
@@ -3580,9 +3496,9 @@
       <c r="H75" s="5"/>
     </row>
     <row r="76" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A76" s="13"/>
-      <c r="B76" s="13"/>
-      <c r="C76" s="13"/>
+      <c r="A76" s="14"/>
+      <c r="B76" s="14"/>
+      <c r="C76" s="14"/>
       <c r="D76" s="5" t="s">
         <v>191</v>
       </c>
@@ -3598,9 +3514,9 @@
       <c r="H76" s="5"/>
     </row>
     <row r="77" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A77" s="13"/>
-      <c r="B77" s="13"/>
-      <c r="C77" s="13"/>
+      <c r="A77" s="14"/>
+      <c r="B77" s="14"/>
+      <c r="C77" s="14"/>
       <c r="D77" s="5" t="s">
         <v>193</v>
       </c>
@@ -3616,9 +3532,9 @@
       <c r="H77" s="5"/>
     </row>
     <row r="78" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A78" s="13"/>
-      <c r="B78" s="13"/>
-      <c r="C78" s="14"/>
+      <c r="A78" s="14"/>
+      <c r="B78" s="14"/>
+      <c r="C78" s="15"/>
       <c r="D78" s="5" t="s">
         <v>194</v>
       </c>
@@ -3634,9 +3550,9 @@
       <c r="H78" s="5"/>
     </row>
     <row r="79" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="13"/>
-      <c r="B79" s="13"/>
-      <c r="C79" s="12" t="s">
+      <c r="A79" s="14"/>
+      <c r="B79" s="14"/>
+      <c r="C79" s="13" t="s">
         <v>178</v>
       </c>
       <c r="D79" s="5" t="s">
@@ -3654,9 +3570,9 @@
       <c r="H79" s="5"/>
     </row>
     <row r="80" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A80" s="13"/>
-      <c r="B80" s="13"/>
-      <c r="C80" s="13"/>
+      <c r="A80" s="14"/>
+      <c r="B80" s="14"/>
+      <c r="C80" s="14"/>
       <c r="D80" s="5" t="s">
         <v>196</v>
       </c>
@@ -3672,9 +3588,9 @@
       <c r="H80" s="5"/>
     </row>
     <row r="81" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A81" s="13"/>
-      <c r="B81" s="13"/>
-      <c r="C81" s="13"/>
+      <c r="A81" s="14"/>
+      <c r="B81" s="14"/>
+      <c r="C81" s="14"/>
       <c r="D81" s="5" t="s">
         <v>197</v>
       </c>
@@ -3690,9 +3606,9 @@
       <c r="H81" s="5"/>
     </row>
     <row r="82" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A82" s="13"/>
-      <c r="B82" s="13"/>
-      <c r="C82" s="13"/>
+      <c r="A82" s="14"/>
+      <c r="B82" s="14"/>
+      <c r="C82" s="14"/>
       <c r="D82" s="5" t="s">
         <v>198</v>
       </c>
@@ -3708,9 +3624,9 @@
       <c r="H82" s="5"/>
     </row>
     <row r="83" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A83" s="13"/>
-      <c r="B83" s="13"/>
-      <c r="C83" s="13"/>
+      <c r="A83" s="14"/>
+      <c r="B83" s="14"/>
+      <c r="C83" s="14"/>
       <c r="D83" s="5" t="s">
         <v>199</v>
       </c>
@@ -3726,9 +3642,9 @@
       <c r="H83" s="5"/>
     </row>
     <row r="84" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A84" s="13"/>
-      <c r="B84" s="13"/>
-      <c r="C84" s="13"/>
+      <c r="A84" s="14"/>
+      <c r="B84" s="14"/>
+      <c r="C84" s="14"/>
       <c r="D84" s="5" t="s">
         <v>200</v>
       </c>
@@ -3744,7 +3660,7 @@
       <c r="H84" s="5"/>
     </row>
     <row r="85" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A85" s="12" t="s">
+      <c r="A85" s="13" t="s">
         <v>187</v>
       </c>
       <c r="B85" s="3" t="s">
@@ -3768,11 +3684,11 @@
       <c r="H85" s="5"/>
     </row>
     <row r="86" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="13"/>
-      <c r="B86" s="12" t="s">
+      <c r="A86" s="14"/>
+      <c r="B86" s="13" t="s">
         <v>211</v>
       </c>
-      <c r="C86" s="15" t="s">
+      <c r="C86" s="16" t="s">
         <v>203</v>
       </c>
       <c r="D86" s="5" t="s">
@@ -3790,9 +3706,9 @@
       <c r="H86" s="5"/>
     </row>
     <row r="87" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A87" s="13"/>
-      <c r="B87" s="13"/>
-      <c r="C87" s="15"/>
+      <c r="A87" s="14"/>
+      <c r="B87" s="14"/>
+      <c r="C87" s="16"/>
       <c r="D87" s="5" t="s">
         <v>220</v>
       </c>
@@ -3808,9 +3724,9 @@
       <c r="H87" s="5"/>
     </row>
     <row r="88" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A88" s="13"/>
-      <c r="B88" s="13"/>
-      <c r="C88" s="15"/>
+      <c r="A88" s="14"/>
+      <c r="B88" s="14"/>
+      <c r="C88" s="16"/>
       <c r="D88" s="5" t="s">
         <v>221</v>
       </c>
@@ -3826,9 +3742,9 @@
       <c r="H88" s="5"/>
     </row>
     <row r="89" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A89" s="13"/>
-      <c r="B89" s="13"/>
-      <c r="C89" s="15"/>
+      <c r="A89" s="14"/>
+      <c r="B89" s="14"/>
+      <c r="C89" s="16"/>
       <c r="D89" s="5" t="s">
         <v>222</v>
       </c>
@@ -3844,9 +3760,9 @@
       <c r="H89" s="5"/>
     </row>
     <row r="90" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A90" s="13"/>
-      <c r="B90" s="13"/>
-      <c r="C90" s="15"/>
+      <c r="A90" s="14"/>
+      <c r="B90" s="14"/>
+      <c r="C90" s="16"/>
       <c r="D90" s="5" t="s">
         <v>228</v>
       </c>
@@ -3862,9 +3778,9 @@
       <c r="H90" s="5"/>
     </row>
     <row r="91" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A91" s="13"/>
-      <c r="B91" s="13"/>
-      <c r="C91" s="15"/>
+      <c r="A91" s="14"/>
+      <c r="B91" s="14"/>
+      <c r="C91" s="16"/>
       <c r="D91" s="5" t="s">
         <v>229</v>
       </c>
@@ -3880,9 +3796,9 @@
       <c r="H91" s="5"/>
     </row>
     <row r="92" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A92" s="14"/>
-      <c r="B92" s="14"/>
-      <c r="C92" s="15"/>
+      <c r="A92" s="15"/>
+      <c r="B92" s="15"/>
+      <c r="C92" s="16"/>
       <c r="D92" s="5" t="s">
         <v>230</v>
       </c>
@@ -3898,13 +3814,13 @@
       <c r="H92" s="5"/>
     </row>
     <row r="93" spans="1:8" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="12" t="s">
+      <c r="A93" s="13" t="s">
         <v>212</v>
       </c>
-      <c r="B93" s="12" t="s">
+      <c r="B93" s="13" t="s">
         <v>213</v>
       </c>
-      <c r="C93" s="12" t="s">
+      <c r="C93" s="13" t="s">
         <v>236</v>
       </c>
       <c r="D93" s="5" t="s">
@@ -3922,9 +3838,9 @@
       <c r="H93" s="5"/>
     </row>
     <row r="94" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A94" s="13"/>
-      <c r="B94" s="13"/>
-      <c r="C94" s="13"/>
+      <c r="A94" s="14"/>
+      <c r="B94" s="14"/>
+      <c r="C94" s="14"/>
       <c r="D94" s="5" t="s">
         <v>232</v>
       </c>
@@ -3940,9 +3856,9 @@
       <c r="H94" s="5"/>
     </row>
     <row r="95" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A95" s="13"/>
-      <c r="B95" s="13"/>
-      <c r="C95" s="13"/>
+      <c r="A95" s="14"/>
+      <c r="B95" s="14"/>
+      <c r="C95" s="14"/>
       <c r="D95" s="5" t="s">
         <v>239</v>
       </c>
@@ -3958,9 +3874,9 @@
       <c r="H95" s="5"/>
     </row>
     <row r="96" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A96" s="13"/>
-      <c r="B96" s="13"/>
-      <c r="C96" s="13"/>
+      <c r="A96" s="14"/>
+      <c r="B96" s="14"/>
+      <c r="C96" s="14"/>
       <c r="D96" s="5" t="s">
         <v>243</v>
       </c>
@@ -3976,9 +3892,9 @@
       <c r="H96" s="5"/>
     </row>
     <row r="97" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A97" s="13"/>
-      <c r="B97" s="13"/>
-      <c r="C97" s="13"/>
+      <c r="A97" s="14"/>
+      <c r="B97" s="14"/>
+      <c r="C97" s="14"/>
       <c r="D97" s="5" t="s">
         <v>247</v>
       </c>
@@ -3994,9 +3910,9 @@
       <c r="H97" s="5"/>
     </row>
     <row r="98" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A98" s="13"/>
-      <c r="B98" s="13"/>
-      <c r="C98" s="13"/>
+      <c r="A98" s="14"/>
+      <c r="B98" s="14"/>
+      <c r="C98" s="14"/>
       <c r="D98" s="5" t="s">
         <v>248</v>
       </c>
@@ -4012,9 +3928,9 @@
       <c r="H98" s="5"/>
     </row>
     <row r="99" spans="1:8" ht="135" x14ac:dyDescent="0.25">
-      <c r="A99" s="13"/>
-      <c r="B99" s="13"/>
-      <c r="C99" s="13"/>
+      <c r="A99" s="14"/>
+      <c r="B99" s="14"/>
+      <c r="C99" s="14"/>
       <c r="D99" s="5" t="s">
         <v>249</v>
       </c>
@@ -4030,9 +3946,9 @@
       <c r="H99" s="5"/>
     </row>
     <row r="100" spans="1:8" ht="120" x14ac:dyDescent="0.25">
-      <c r="A100" s="13"/>
-      <c r="B100" s="13"/>
-      <c r="C100" s="13"/>
+      <c r="A100" s="14"/>
+      <c r="B100" s="14"/>
+      <c r="C100" s="14"/>
       <c r="D100" s="5" t="s">
         <v>250</v>
       </c>
@@ -4050,13 +3966,13 @@
       </c>
     </row>
     <row r="101" spans="1:8" ht="105" x14ac:dyDescent="0.25">
-      <c r="A101" s="13"/>
-      <c r="B101" s="13"/>
-      <c r="C101" s="13"/>
+      <c r="A101" s="14"/>
+      <c r="B101" s="14"/>
+      <c r="C101" s="14"/>
       <c r="D101" s="5" t="s">
         <v>251</v>
       </c>
-      <c r="E101" s="16" t="s">
+      <c r="E101" s="12" t="s">
         <v>234</v>
       </c>
       <c r="F101" s="3" t="s">
@@ -4068,13 +3984,13 @@
       <c r="H101" s="5"/>
     </row>
     <row r="102" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A102" s="13"/>
-      <c r="B102" s="13"/>
-      <c r="C102" s="13"/>
+      <c r="A102" s="14"/>
+      <c r="B102" s="14"/>
+      <c r="C102" s="14"/>
       <c r="D102" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="E102" s="16" t="s">
+      <c r="E102" s="12" t="s">
         <v>237</v>
       </c>
       <c r="F102" s="3" t="s">
@@ -4088,9 +4004,9 @@
       </c>
     </row>
     <row r="103" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A103" s="13"/>
-      <c r="B103" s="13"/>
-      <c r="C103" s="13"/>
+      <c r="A103" s="14"/>
+      <c r="B103" s="14"/>
+      <c r="C103" s="14"/>
       <c r="D103" s="5" t="s">
         <v>253</v>
       </c>
@@ -4106,9 +4022,9 @@
       <c r="H103" s="5"/>
     </row>
     <row r="104" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A104" s="13"/>
-      <c r="B104" s="13"/>
-      <c r="C104" s="13"/>
+      <c r="A104" s="14"/>
+      <c r="B104" s="14"/>
+      <c r="C104" s="14"/>
       <c r="D104" s="5" t="s">
         <v>266</v>
       </c>
@@ -4124,9 +4040,9 @@
       <c r="H104" s="5"/>
     </row>
     <row r="105" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A105" s="14"/>
-      <c r="B105" s="14"/>
-      <c r="C105" s="14"/>
+      <c r="A105" s="15"/>
+      <c r="B105" s="15"/>
+      <c r="C105" s="15"/>
       <c r="D105" s="5" t="s">
         <v>267</v>
       </c>
@@ -4142,7 +4058,7 @@
       <c r="H105" s="5"/>
     </row>
     <row r="106" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A106" s="12" t="s">
+      <c r="A106" s="13" t="s">
         <v>244</v>
       </c>
       <c r="B106" s="3" t="s">
@@ -4166,11 +4082,11 @@
       <c r="H106" s="5"/>
     </row>
     <row r="107" spans="1:8" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="13"/>
-      <c r="B107" s="12" t="s">
+      <c r="A107" s="14"/>
+      <c r="B107" s="13" t="s">
         <v>256</v>
       </c>
-      <c r="C107" s="12" t="s">
+      <c r="C107" s="13" t="s">
         <v>262</v>
       </c>
       <c r="D107" s="5" t="s">
@@ -4188,9 +4104,9 @@
       <c r="H107" s="5"/>
     </row>
     <row r="108" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A108" s="13"/>
-      <c r="B108" s="13"/>
-      <c r="C108" s="13"/>
+      <c r="A108" s="14"/>
+      <c r="B108" s="14"/>
+      <c r="C108" s="14"/>
       <c r="D108" s="5" t="s">
         <v>273</v>
       </c>
@@ -4206,9 +4122,9 @@
       <c r="H108" s="5"/>
     </row>
     <row r="109" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A109" s="13"/>
-      <c r="B109" s="13"/>
-      <c r="C109" s="13"/>
+      <c r="A109" s="14"/>
+      <c r="B109" s="14"/>
+      <c r="C109" s="14"/>
       <c r="D109" s="5" t="s">
         <v>275</v>
       </c>
@@ -4224,9 +4140,9 @@
       <c r="H109" s="5"/>
     </row>
     <row r="110" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A110" s="13"/>
-      <c r="B110" s="13"/>
-      <c r="C110" s="13"/>
+      <c r="A110" s="14"/>
+      <c r="B110" s="14"/>
+      <c r="C110" s="14"/>
       <c r="D110" s="5" t="s">
         <v>276</v>
       </c>
@@ -4242,9 +4158,9 @@
       <c r="H110" s="5"/>
     </row>
     <row r="111" spans="1:8" ht="135" x14ac:dyDescent="0.25">
-      <c r="A111" s="13"/>
-      <c r="B111" s="13"/>
-      <c r="C111" s="13"/>
+      <c r="A111" s="14"/>
+      <c r="B111" s="14"/>
+      <c r="C111" s="14"/>
       <c r="D111" s="5" t="s">
         <v>277</v>
       </c>
@@ -4260,9 +4176,9 @@
       <c r="H111" s="5"/>
     </row>
     <row r="112" spans="1:8" ht="120" x14ac:dyDescent="0.25">
-      <c r="A112" s="13"/>
-      <c r="B112" s="13"/>
-      <c r="C112" s="13"/>
+      <c r="A112" s="14"/>
+      <c r="B112" s="14"/>
+      <c r="C112" s="14"/>
       <c r="D112" s="5" t="s">
         <v>278</v>
       </c>
@@ -4280,9 +4196,9 @@
       </c>
     </row>
     <row r="113" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A113" s="13"/>
-      <c r="B113" s="13"/>
-      <c r="C113" s="13"/>
+      <c r="A113" s="14"/>
+      <c r="B113" s="14"/>
+      <c r="C113" s="14"/>
       <c r="D113" s="5" t="s">
         <v>279</v>
       </c>
@@ -4298,9 +4214,9 @@
       <c r="H113" s="5"/>
     </row>
     <row r="114" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A114" s="13"/>
-      <c r="B114" s="13"/>
-      <c r="C114" s="13"/>
+      <c r="A114" s="14"/>
+      <c r="B114" s="14"/>
+      <c r="C114" s="14"/>
       <c r="D114" s="5" t="s">
         <v>287</v>
       </c>
@@ -4316,9 +4232,9 @@
       <c r="H114" s="5"/>
     </row>
     <row r="115" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A115" s="13"/>
-      <c r="B115" s="13"/>
-      <c r="C115" s="13"/>
+      <c r="A115" s="14"/>
+      <c r="B115" s="14"/>
+      <c r="C115" s="14"/>
       <c r="D115" s="5" t="s">
         <v>293</v>
       </c>
@@ -4334,9 +4250,9 @@
       <c r="H115" s="5"/>
     </row>
     <row r="116" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A116" s="13"/>
-      <c r="B116" s="13"/>
-      <c r="C116" s="13"/>
+      <c r="A116" s="14"/>
+      <c r="B116" s="14"/>
+      <c r="C116" s="14"/>
       <c r="D116" s="5" t="s">
         <v>298</v>
       </c>
@@ -4352,9 +4268,9 @@
       <c r="H116" s="5"/>
     </row>
     <row r="117" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A117" s="13"/>
-      <c r="B117" s="13"/>
-      <c r="C117" s="13"/>
+      <c r="A117" s="14"/>
+      <c r="B117" s="14"/>
+      <c r="C117" s="14"/>
       <c r="D117" s="5" t="s">
         <v>317</v>
       </c>
@@ -4370,9 +4286,9 @@
       <c r="H117" s="5"/>
     </row>
     <row r="118" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A118" s="13"/>
-      <c r="B118" s="13"/>
-      <c r="C118" s="13"/>
+      <c r="A118" s="14"/>
+      <c r="B118" s="14"/>
+      <c r="C118" s="14"/>
       <c r="D118" s="5" t="s">
         <v>318</v>
       </c>
@@ -4388,9 +4304,9 @@
       <c r="H118" s="5"/>
     </row>
     <row r="119" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A119" s="13"/>
-      <c r="B119" s="13"/>
-      <c r="C119" s="13"/>
+      <c r="A119" s="14"/>
+      <c r="B119" s="14"/>
+      <c r="C119" s="14"/>
       <c r="D119" s="5" t="s">
         <v>319</v>
       </c>
@@ -4406,9 +4322,9 @@
       <c r="H119" s="5"/>
     </row>
     <row r="120" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A120" s="13"/>
-      <c r="B120" s="13"/>
-      <c r="C120" s="13"/>
+      <c r="A120" s="14"/>
+      <c r="B120" s="14"/>
+      <c r="C120" s="14"/>
       <c r="D120" s="5" t="s">
         <v>320</v>
       </c>
@@ -4424,9 +4340,9 @@
       <c r="H120" s="5"/>
     </row>
     <row r="121" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A121" s="13"/>
-      <c r="B121" s="13"/>
-      <c r="C121" s="13"/>
+      <c r="A121" s="14"/>
+      <c r="B121" s="14"/>
+      <c r="C121" s="14"/>
       <c r="D121" s="5" t="s">
         <v>321</v>
       </c>
@@ -4442,9 +4358,9 @@
       <c r="H121" s="5"/>
     </row>
     <row r="122" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A122" s="13"/>
-      <c r="B122" s="14"/>
-      <c r="C122" s="14"/>
+      <c r="A122" s="14"/>
+      <c r="B122" s="15"/>
+      <c r="C122" s="15"/>
       <c r="D122" s="5" t="s">
         <v>333</v>
       </c>
@@ -4460,7 +4376,7 @@
       <c r="H122" s="5"/>
     </row>
     <row r="123" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A123" s="14"/>
+      <c r="A123" s="15"/>
       <c r="B123" s="3" t="s">
         <v>285</v>
       </c>
@@ -4482,7 +4398,7 @@
       <c r="H123" s="5"/>
     </row>
     <row r="124" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A124" s="15" t="s">
+      <c r="A124" s="16" t="s">
         <v>290</v>
       </c>
       <c r="B124" s="3" t="s">
@@ -4506,7 +4422,7 @@
       <c r="H124" s="5"/>
     </row>
     <row r="125" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A125" s="15"/>
+      <c r="A125" s="16"/>
       <c r="B125" s="3" t="s">
         <v>296</v>
       </c>
@@ -4545,6 +4461,9 @@
     <mergeCell ref="A85:A92"/>
     <mergeCell ref="C79:C84"/>
     <mergeCell ref="B72:B84"/>
+    <mergeCell ref="A28:A34"/>
+    <mergeCell ref="B28:B34"/>
+    <mergeCell ref="C28:C34"/>
     <mergeCell ref="A72:A84"/>
     <mergeCell ref="C35:C45"/>
     <mergeCell ref="B35:B45"/>
@@ -4558,167 +4477,164 @@
     <mergeCell ref="A35:A71"/>
     <mergeCell ref="C53:C59"/>
     <mergeCell ref="B53:B59"/>
-    <mergeCell ref="A28:A34"/>
-    <mergeCell ref="B28:B34"/>
-    <mergeCell ref="C28:C34"/>
   </mergeCells>
   <conditionalFormatting sqref="G50:G56 G58:G87 G92:G103 G107:G1048576 G28:G34 G1:G20">
-    <cfRule type="cellIs" dxfId="45" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="43" operator="equal">
       <formula>"Falhou"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="44" operator="equal">
       <formula>"Passou"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G58:G63 G35:G56">
-    <cfRule type="cellIs" dxfId="43" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="41" operator="equal">
       <formula>"Falhou"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="42" operator="equal">
       <formula>"Passou"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G57">
-    <cfRule type="cellIs" dxfId="41" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="39" operator="equal">
       <formula>"Falhou"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="40" operator="equal">
       <formula>"Passou"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G88">
-    <cfRule type="cellIs" dxfId="39" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="37" operator="equal">
       <formula>"Falhou"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="38" operator="equal">
       <formula>"Passou"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G89">
-    <cfRule type="cellIs" dxfId="37" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="35" operator="equal">
       <formula>"Falhou"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="36" operator="equal">
       <formula>"Passou"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G90">
-    <cfRule type="cellIs" dxfId="35" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="33" operator="equal">
       <formula>"Falhou"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="34" operator="equal">
       <formula>"Passou"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G91">
-    <cfRule type="cellIs" dxfId="33" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="31" operator="equal">
       <formula>"Falhou"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="32" operator="equal">
       <formula>"Passou"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G91">
-    <cfRule type="cellIs" dxfId="31" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="29" operator="equal">
       <formula>"Falhou"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="30" operator="equal">
       <formula>"Passou"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G92:G99">
-    <cfRule type="cellIs" dxfId="29" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="27" operator="equal">
       <formula>"Falhou"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="28" operator="equal">
       <formula>"Passou"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G104">
-    <cfRule type="cellIs" dxfId="27" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="25" operator="equal">
       <formula>"Falhou"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="26" operator="equal">
       <formula>"Passou"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G104">
-    <cfRule type="cellIs" dxfId="25" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="23" operator="equal">
       <formula>"Falhou"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="24" operator="equal">
       <formula>"Passou"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G105:G106">
-    <cfRule type="cellIs" dxfId="23" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="21" operator="equal">
       <formula>"Falhou"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="22" operator="equal">
       <formula>"Passou"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G105:G106">
-    <cfRule type="cellIs" dxfId="21" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="19" operator="equal">
       <formula>"Falhou"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="20" operator="equal">
       <formula>"Passou"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G103">
-    <cfRule type="cellIs" dxfId="17" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="13" operator="equal">
       <formula>"Falhou"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="14" operator="equal">
       <formula>"Passou"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G103">
-    <cfRule type="cellIs" dxfId="13" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
       <formula>"Falhou"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
       <formula>"Passou"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G104">
-    <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
       <formula>"Falhou"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
       <formula>"Passou"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G104">
-    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
       <formula>"Falhou"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
       <formula>"Passou"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G105:G106">
-    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>"Falhou"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
       <formula>"Passou"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G105:G106">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"Falhou"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>"Passou"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G21:G27">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Falhou"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"Passou"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>